<commit_message>
promise api oops added and html css added
</commit_message>
<xml_diff>
--- a/JS_React_Syllabus.xlsx
+++ b/JS_React_Syllabus.xlsx
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
   <si>
     <t>Day</t>
   </si>
@@ -237,6 +238,30 @@
   </si>
   <si>
     <t>TypeScript</t>
+  </si>
+  <si>
+    <t>v8</t>
+  </si>
+  <si>
+    <t>start</t>
+  </si>
+  <si>
+    <t>end</t>
+  </si>
+  <si>
+    <t>browser</t>
+  </si>
+  <si>
+    <t>event loop</t>
+  </si>
+  <si>
+    <t>file read</t>
+  </si>
+  <si>
+    <t>processing the data</t>
+  </si>
+  <si>
+    <t>sync</t>
   </si>
 </sst>
 </file>
@@ -280,7 +305,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -292,10 +317,17 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -579,8 +611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -602,74 +634,74 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="8" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="2" t="s">
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="8" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="2" t="s">
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="8" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="8" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="2" t="s">
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="8" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="2" t="s">
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="8" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="2" t="s">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="8" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="2" t="s">
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="8" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="5" t="s">
         <v>33</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -677,38 +709,38 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
       <c r="C11" s="2" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
       <c r="C12" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
       <c r="C13" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
       <c r="C14" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C15" s="2" t="s">
@@ -716,38 +748,38 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
       <c r="C16" s="2" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
       <c r="C17" s="2" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
       <c r="C18" s="2" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
       <c r="C19" s="2" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C20" s="2" t="s">
@@ -755,31 +787,31 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
       <c r="C21" s="2" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
       <c r="C22" s="2" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
       <c r="C23" s="2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="5" t="s">
         <v>45</v>
       </c>
       <c r="C24" s="2" t="s">
@@ -787,38 +819,38 @@
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
       <c r="C25" s="2" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="4"/>
-      <c r="B26" s="4"/>
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
       <c r="C26" s="2" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="4"/>
-      <c r="B27" s="4"/>
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
       <c r="C27" s="2" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="4"/>
-      <c r="B28" s="4"/>
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
       <c r="C28" s="2" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="4" t="s">
+      <c r="A29" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="5" t="s">
         <v>51</v>
       </c>
       <c r="C29" s="2" t="s">
@@ -826,17 +858,17 @@
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="4"/>
-      <c r="B30" s="4"/>
+      <c r="A30" s="5"/>
+      <c r="B30" s="5"/>
       <c r="C30" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="4" t="s">
+      <c r="A31" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="5" t="s">
         <v>54</v>
       </c>
       <c r="C31" s="2" t="s">
@@ -844,31 +876,31 @@
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" s="4"/>
-      <c r="B32" s="4"/>
+      <c r="A32" s="5"/>
+      <c r="B32" s="5"/>
       <c r="C32" s="2" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" s="4"/>
-      <c r="B33" s="4"/>
+      <c r="A33" s="5"/>
+      <c r="B33" s="5"/>
       <c r="C33" s="2" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" s="4"/>
-      <c r="B34" s="4"/>
+      <c r="A34" s="5"/>
+      <c r="B34" s="5"/>
       <c r="C34" s="2" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="4" t="s">
+      <c r="A35" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B35" s="5" t="s">
         <v>59</v>
       </c>
       <c r="C35" s="2" t="s">
@@ -876,24 +908,24 @@
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" s="4"/>
-      <c r="B36" s="4"/>
+      <c r="A36" s="5"/>
+      <c r="B36" s="5"/>
       <c r="C36" s="2" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="4"/>
-      <c r="B37" s="4"/>
+      <c r="A37" s="5"/>
+      <c r="B37" s="5"/>
       <c r="C37" s="2" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" s="4" t="s">
+      <c r="A38" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B38" s="5" t="s">
         <v>63</v>
       </c>
       <c r="C38" s="2" t="s">
@@ -901,15 +933,15 @@
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" s="4"/>
-      <c r="B39" s="4"/>
+      <c r="A39" s="5"/>
+      <c r="B39" s="5"/>
       <c r="C39" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" s="4"/>
-      <c r="B40" s="4"/>
+      <c r="A40" s="5"/>
+      <c r="B40" s="5"/>
       <c r="C40" s="2" t="s">
         <v>22</v>
       </c>
@@ -940,7 +972,7 @@
       <c r="A43" t="s">
         <v>68</v>
       </c>
-      <c r="B43" s="5" t="s">
+      <c r="B43" s="4" t="s">
         <v>69</v>
       </c>
       <c r="C43" s="2" t="s">
@@ -949,6 +981,18 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="A5:A9"/>
+    <mergeCell ref="B5:B9"/>
+    <mergeCell ref="A10:A14"/>
+    <mergeCell ref="B10:B14"/>
+    <mergeCell ref="A15:A19"/>
+    <mergeCell ref="B15:B19"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="B20:B23"/>
+    <mergeCell ref="A24:A28"/>
+    <mergeCell ref="B24:B28"/>
     <mergeCell ref="A38:A40"/>
     <mergeCell ref="B38:B40"/>
     <mergeCell ref="A29:A30"/>
@@ -957,19 +1001,81 @@
     <mergeCell ref="B31:B34"/>
     <mergeCell ref="A35:A37"/>
     <mergeCell ref="B35:B37"/>
-    <mergeCell ref="A15:A19"/>
-    <mergeCell ref="B15:B19"/>
-    <mergeCell ref="A20:A23"/>
-    <mergeCell ref="B20:B23"/>
-    <mergeCell ref="A24:A28"/>
-    <mergeCell ref="B24:B28"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="A5:A9"/>
-    <mergeCell ref="B5:B9"/>
-    <mergeCell ref="A10:A14"/>
-    <mergeCell ref="B10:B14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A6:D20"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C8" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>73</v>
+      </c>
+      <c r="D12">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>71</v>
+      </c>
+      <c r="D14" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C18">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C20" t="s">
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
syllabus completion updated, classwork-2 answers added
</commit_message>
<xml_diff>
--- a/JS_React_Syllabus.xlsx
+++ b/JS_React_Syllabus.xlsx
@@ -319,15 +319,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -612,7 +612,7 @@
   <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:A14"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -640,21 +640,21 @@
       <c r="B2" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="6" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="7"/>
       <c r="B3" s="7"/>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="6" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="7"/>
       <c r="B4" s="7"/>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="6" t="s">
         <v>29</v>
       </c>
     </row>
@@ -665,82 +665,82 @@
       <c r="B5" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="6" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="6" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="6" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="6" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="6" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="2" t="s">
+      <c r="A11" s="8"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="6" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="2" t="s">
+      <c r="A12" s="8"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="2" t="s">
+      <c r="A13" s="8"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="6" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
+      <c r="A14" s="8"/>
+      <c r="B14" s="8"/>
       <c r="C14" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C15" s="2" t="s">
@@ -748,38 +748,38 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
+      <c r="A16" s="8"/>
+      <c r="B16" s="8"/>
       <c r="C16" s="2" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
+      <c r="A17" s="8"/>
+      <c r="B17" s="8"/>
       <c r="C17" s="2" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
+      <c r="A18" s="8"/>
+      <c r="B18" s="8"/>
       <c r="C18" s="2" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
+      <c r="A19" s="8"/>
+      <c r="B19" s="8"/>
       <c r="C19" s="2" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="8" t="s">
         <v>8</v>
       </c>
       <c r="C20" s="2" t="s">
@@ -787,31 +787,31 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
+      <c r="A21" s="8"/>
+      <c r="B21" s="8"/>
       <c r="C21" s="2" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
+      <c r="A22" s="8"/>
+      <c r="B22" s="8"/>
       <c r="C22" s="2" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="5"/>
-      <c r="B23" s="5"/>
+      <c r="A23" s="8"/>
+      <c r="B23" s="8"/>
       <c r="C23" s="2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="5" t="s">
+      <c r="A24" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="8" t="s">
         <v>45</v>
       </c>
       <c r="C24" s="2" t="s">
@@ -819,38 +819,38 @@
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
+      <c r="A25" s="8"/>
+      <c r="B25" s="8"/>
       <c r="C25" s="2" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="5"/>
-      <c r="B26" s="5"/>
+      <c r="A26" s="8"/>
+      <c r="B26" s="8"/>
       <c r="C26" s="2" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="5"/>
-      <c r="B27" s="5"/>
+      <c r="A27" s="8"/>
+      <c r="B27" s="8"/>
       <c r="C27" s="2" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="5"/>
-      <c r="B28" s="5"/>
+      <c r="A28" s="8"/>
+      <c r="B28" s="8"/>
       <c r="C28" s="2" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="5" t="s">
+      <c r="A29" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B29" s="8" t="s">
         <v>51</v>
       </c>
       <c r="C29" s="2" t="s">
@@ -858,17 +858,17 @@
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="5"/>
-      <c r="B30" s="5"/>
+      <c r="A30" s="8"/>
+      <c r="B30" s="8"/>
       <c r="C30" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="5" t="s">
+      <c r="A31" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B31" s="8" t="s">
         <v>54</v>
       </c>
       <c r="C31" s="2" t="s">
@@ -876,31 +876,31 @@
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" s="5"/>
-      <c r="B32" s="5"/>
+      <c r="A32" s="8"/>
+      <c r="B32" s="8"/>
       <c r="C32" s="2" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" s="5"/>
-      <c r="B33" s="5"/>
+      <c r="A33" s="8"/>
+      <c r="B33" s="8"/>
       <c r="C33" s="2" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" s="5"/>
-      <c r="B34" s="5"/>
+      <c r="A34" s="8"/>
+      <c r="B34" s="8"/>
       <c r="C34" s="2" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="5" t="s">
+      <c r="A35" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B35" s="8" t="s">
         <v>59</v>
       </c>
       <c r="C35" s="2" t="s">
@@ -908,24 +908,24 @@
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" s="5"/>
-      <c r="B36" s="5"/>
+      <c r="A36" s="8"/>
+      <c r="B36" s="8"/>
       <c r="C36" s="2" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="5"/>
-      <c r="B37" s="5"/>
+      <c r="A37" s="8"/>
+      <c r="B37" s="8"/>
       <c r="C37" s="2" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" s="5" t="s">
+      <c r="A38" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B38" s="8" t="s">
         <v>63</v>
       </c>
       <c r="C38" s="2" t="s">
@@ -933,15 +933,15 @@
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" s="5"/>
-      <c r="B39" s="5"/>
+      <c r="A39" s="8"/>
+      <c r="B39" s="8"/>
       <c r="C39" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" s="5"/>
-      <c r="B40" s="5"/>
+      <c r="A40" s="8"/>
+      <c r="B40" s="8"/>
       <c r="C40" s="2" t="s">
         <v>22</v>
       </c>
@@ -981,18 +981,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="A5:A9"/>
-    <mergeCell ref="B5:B9"/>
-    <mergeCell ref="A10:A14"/>
-    <mergeCell ref="B10:B14"/>
-    <mergeCell ref="A15:A19"/>
-    <mergeCell ref="B15:B19"/>
-    <mergeCell ref="A20:A23"/>
-    <mergeCell ref="B20:B23"/>
-    <mergeCell ref="A24:A28"/>
-    <mergeCell ref="B24:B28"/>
     <mergeCell ref="A38:A40"/>
     <mergeCell ref="B38:B40"/>
     <mergeCell ref="A29:A30"/>
@@ -1001,8 +989,21 @@
     <mergeCell ref="B31:B34"/>
     <mergeCell ref="A35:A37"/>
     <mergeCell ref="B35:B37"/>
+    <mergeCell ref="A15:A19"/>
+    <mergeCell ref="B15:B19"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="B20:B23"/>
+    <mergeCell ref="A24:A28"/>
+    <mergeCell ref="B24:B28"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="A5:A9"/>
+    <mergeCell ref="B5:B9"/>
+    <mergeCell ref="A10:A14"/>
+    <mergeCell ref="B10:B14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1020,7 +1021,7 @@
       <c r="A6">
         <v>1</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>72</v>
       </c>
     </row>

</xml_diff>

<commit_message>
git notes added and api fetch question set added
</commit_message>
<xml_diff>
--- a/JS_React_Syllabus.xlsx
+++ b/JS_React_Syllabus.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
   <si>
     <t>Day</t>
   </si>
@@ -262,6 +262,9 @@
   </si>
   <si>
     <t>sync</t>
+  </si>
+  <si>
+    <t>Version Control: Git and GitHub</t>
   </si>
 </sst>
 </file>
@@ -323,10 +326,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -609,10 +612,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C43"/>
+  <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -634,10 +637,10 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="8" t="s">
         <v>26</v>
       </c>
       <c r="C2" s="6" t="s">
@@ -645,24 +648,24 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
       <c r="C3" s="6" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
+      <c r="A4" s="8"/>
+      <c r="B4" s="8"/>
       <c r="C4" s="6" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="8" t="s">
         <v>30</v>
       </c>
       <c r="C5" s="6" t="s">
@@ -670,29 +673,29 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
+      <c r="A6" s="8"/>
+      <c r="B6" s="8"/>
       <c r="C6" s="6" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
+      <c r="A7" s="8"/>
+      <c r="B7" s="8"/>
       <c r="C7" s="6" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
+      <c r="A8" s="8"/>
+      <c r="B8" s="8"/>
       <c r="C8" s="6" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
+      <c r="A9" s="8"/>
+      <c r="B9" s="8"/>
       <c r="C9" s="6" t="s">
         <v>32</v>
       </c>
@@ -737,10 +740,10 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C15" s="2" t="s">
@@ -748,259 +751,266 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
+      <c r="A16" s="7"/>
+      <c r="B16" s="7"/>
       <c r="C16" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="7"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="2" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="2" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="7"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="8"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="2" t="s">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="7"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="8" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B21" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C21" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="8"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="2" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="7"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="8"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="2" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="7"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="8"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="2" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="7"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="8" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B25" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C25" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="8"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="2" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="7"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="8"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="2" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="7"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="8"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="2" t="s">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="7"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="8"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="2" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="7"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="8" t="s">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="B30" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C30" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="8"/>
-      <c r="B30" s="8"/>
-      <c r="C30" s="2" t="s">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="7"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="8" t="s">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="B32" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C32" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" s="8"/>
-      <c r="B32" s="8"/>
-      <c r="C32" s="2" t="s">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="7"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" s="8"/>
-      <c r="B33" s="8"/>
-      <c r="C33" s="2" t="s">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="7"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" s="8"/>
-      <c r="B34" s="8"/>
-      <c r="C34" s="2" t="s">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="7"/>
+      <c r="B35" s="7"/>
+      <c r="C35" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="8" t="s">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B35" s="8" t="s">
+      <c r="B36" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C36" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" s="8"/>
-      <c r="B36" s="8"/>
-      <c r="C36" s="2" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="7"/>
+      <c r="B37" s="7"/>
+      <c r="C37" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="8"/>
-      <c r="B37" s="8"/>
-      <c r="C37" s="2" t="s">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="7"/>
+      <c r="B38" s="7"/>
+      <c r="C38" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" s="8" t="s">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B38" s="8" t="s">
+      <c r="B39" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C39" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" s="8"/>
-      <c r="B39" s="8"/>
-      <c r="C39" s="2" t="s">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" s="7"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" s="8"/>
-      <c r="B40" s="8"/>
-      <c r="C40" s="2" t="s">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" s="7"/>
+      <c r="B41" s="7"/>
+      <c r="C41" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" s="3" t="s">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B42" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="C42" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42" s="2" t="s">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="B43" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="C43" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
         <v>68</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="B44" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="C44" s="2" t="s">
         <v>67</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A38:A40"/>
-    <mergeCell ref="B38:B40"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="A31:A34"/>
-    <mergeCell ref="B31:B34"/>
-    <mergeCell ref="A35:A37"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="A15:A19"/>
-    <mergeCell ref="B15:B19"/>
-    <mergeCell ref="A20:A23"/>
-    <mergeCell ref="B20:B23"/>
-    <mergeCell ref="A24:A28"/>
-    <mergeCell ref="B24:B28"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="A5:A9"/>
     <mergeCell ref="B5:B9"/>
     <mergeCell ref="A10:A14"/>
     <mergeCell ref="B10:B14"/>
+    <mergeCell ref="A15:A20"/>
+    <mergeCell ref="B15:B20"/>
+    <mergeCell ref="A21:A24"/>
+    <mergeCell ref="B21:B24"/>
+    <mergeCell ref="A25:A29"/>
+    <mergeCell ref="B25:B29"/>
+    <mergeCell ref="A39:A41"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="A32:A35"/>
+    <mergeCell ref="B32:B35"/>
+    <mergeCell ref="A36:A38"/>
+    <mergeCell ref="B36:B38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
JS Form classwork question has been added
</commit_message>
<xml_diff>
--- a/JS_React_Syllabus.xlsx
+++ b/JS_React_Syllabus.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="85">
   <si>
     <t>Day</t>
   </si>
@@ -265,6 +265,21 @@
   </si>
   <si>
     <t>Version Control: Git and GitHub</t>
+  </si>
+  <si>
+    <t>Revision HTML and CSS</t>
+  </si>
+  <si>
+    <t>HTML: Introduction, Sementic tags, Emmet Abbreviations</t>
+  </si>
+  <si>
+    <t>CSS: Box Model, Position, Float, Flex</t>
+  </si>
+  <si>
+    <t>CSS: Grid, Transition, Animation</t>
+  </si>
+  <si>
+    <t>CSS: Media Query</t>
   </si>
 </sst>
 </file>
@@ -326,10 +341,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -612,10 +627,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C44"/>
+  <dimension ref="A1:C48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25:B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -637,10 +652,10 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>26</v>
       </c>
       <c r="C2" s="6" t="s">
@@ -648,24 +663,24 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="8"/>
-      <c r="B3" s="8"/>
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
       <c r="C3" s="6" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="8"/>
-      <c r="B4" s="8"/>
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
       <c r="C4" s="6" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>30</v>
       </c>
       <c r="C5" s="6" t="s">
@@ -673,38 +688,38 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="8"/>
-      <c r="B6" s="8"/>
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
       <c r="C6" s="6" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="8"/>
-      <c r="B7" s="8"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
       <c r="C7" s="6" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
       <c r="C8" s="6" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
       <c r="C9" s="6" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="7" t="s">
         <v>33</v>
       </c>
       <c r="C10" s="6" t="s">
@@ -712,29 +727,29 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
       <c r="C11" s="6" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
       <c r="C12" s="6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="8"/>
-      <c r="B13" s="8"/>
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
       <c r="C13" s="6" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
+      <c r="A14" s="7"/>
+      <c r="B14" s="7"/>
       <c r="C14" s="2" t="s">
         <v>19</v>
       </c>
@@ -746,42 +761,42 @@
       <c r="B15" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="6" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="6" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="6" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="6" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="7"/>
       <c r="B20" s="7"/>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="6" t="s">
         <v>40</v>
       </c>
     </row>
@@ -790,227 +805,261 @@
         <v>7</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>41</v>
+        <v>80</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="7"/>
       <c r="B22" s="7"/>
-      <c r="C22" s="2" t="s">
-        <v>42</v>
+      <c r="C22" s="6" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="7"/>
       <c r="B23" s="7"/>
-      <c r="C23" s="2" t="s">
-        <v>43</v>
+      <c r="C23" s="6" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="7"/>
       <c r="B24" s="7"/>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="8"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="8"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="8"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="7" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="B29" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C29" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="7"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="2" t="s">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="8"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="7"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="2" t="s">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="8"/>
+      <c r="B31" s="8"/>
+      <c r="C31" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="7"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="2" t="s">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="8"/>
+      <c r="B32" s="8"/>
+      <c r="C32" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="7"/>
-      <c r="B29" s="7"/>
-      <c r="C29" s="2" t="s">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="8"/>
+      <c r="B33" s="8"/>
+      <c r="C33" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="7" t="s">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B30" s="7" t="s">
+      <c r="B34" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C34" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="7"/>
-      <c r="B31" s="7"/>
-      <c r="C31" s="2" t="s">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="8"/>
+      <c r="B35" s="8"/>
+      <c r="C35" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" s="7" t="s">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B32" s="7" t="s">
+      <c r="B36" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C36" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" s="7"/>
-      <c r="B33" s="7"/>
-      <c r="C33" s="2" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="8"/>
+      <c r="B37" s="8"/>
+      <c r="C37" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" s="7"/>
-      <c r="B34" s="7"/>
-      <c r="C34" s="2" t="s">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="8"/>
+      <c r="B38" s="8"/>
+      <c r="C38" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="7"/>
-      <c r="B35" s="7"/>
-      <c r="C35" s="2" t="s">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="8"/>
+      <c r="B39" s="8"/>
+      <c r="C39" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" s="7" t="s">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B36" s="7" t="s">
+      <c r="B40" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C40" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="7"/>
-      <c r="B37" s="7"/>
-      <c r="C37" s="2" t="s">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" s="8"/>
+      <c r="B41" s="8"/>
+      <c r="C41" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" s="7"/>
-      <c r="B38" s="7"/>
-      <c r="C38" s="2" t="s">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="8"/>
+      <c r="B42" s="8"/>
+      <c r="C42" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" s="7" t="s">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B39" s="7" t="s">
+      <c r="B43" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="C43" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" s="7"/>
-      <c r="B40" s="7"/>
-      <c r="C40" s="2" t="s">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" s="8"/>
+      <c r="B44" s="8"/>
+      <c r="C44" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" s="7"/>
-      <c r="B41" s="7"/>
-      <c r="C41" s="2" t="s">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" s="8"/>
+      <c r="B45" s="8"/>
+      <c r="C45" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42" s="3" t="s">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="B46" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="C46" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43" s="2" t="s">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B47" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="C47" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
         <v>68</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="B48" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C48" s="2" t="s">
         <v>67</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="20">
+  <mergeCells count="22">
+    <mergeCell ref="A43:A45"/>
+    <mergeCell ref="B43:B45"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="B36:B39"/>
+    <mergeCell ref="A40:A42"/>
+    <mergeCell ref="B40:B42"/>
+    <mergeCell ref="A15:A20"/>
+    <mergeCell ref="B15:B20"/>
+    <mergeCell ref="A25:A28"/>
+    <mergeCell ref="B25:B28"/>
+    <mergeCell ref="A29:A33"/>
+    <mergeCell ref="B29:B33"/>
+    <mergeCell ref="A21:A24"/>
+    <mergeCell ref="B21:B24"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="A5:A9"/>
     <mergeCell ref="B5:B9"/>
     <mergeCell ref="A10:A14"/>
     <mergeCell ref="B10:B14"/>
-    <mergeCell ref="A15:A20"/>
-    <mergeCell ref="B15:B20"/>
-    <mergeCell ref="A21:A24"/>
-    <mergeCell ref="B21:B24"/>
-    <mergeCell ref="A25:A29"/>
-    <mergeCell ref="B25:B29"/>
-    <mergeCell ref="A39:A41"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="A32:A35"/>
-    <mergeCell ref="B32:B35"/>
-    <mergeCell ref="A36:A38"/>
-    <mergeCell ref="B36:B38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
classwork JS_map_reduce_filter is added
</commit_message>
<xml_diff>
--- a/JS_React_Syllabus.xlsx
+++ b/JS_React_Syllabus.xlsx
@@ -341,10 +341,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -629,8 +629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25:B28"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -652,10 +652,10 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="8" t="s">
         <v>26</v>
       </c>
       <c r="C2" s="6" t="s">
@@ -663,24 +663,24 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
       <c r="C3" s="6" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
+      <c r="A4" s="8"/>
+      <c r="B4" s="8"/>
       <c r="C4" s="6" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="8" t="s">
         <v>30</v>
       </c>
       <c r="C5" s="6" t="s">
@@ -688,38 +688,38 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
+      <c r="A6" s="8"/>
+      <c r="B6" s="8"/>
       <c r="C6" s="6" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
+      <c r="A7" s="8"/>
+      <c r="B7" s="8"/>
       <c r="C7" s="6" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
+      <c r="A8" s="8"/>
+      <c r="B8" s="8"/>
       <c r="C8" s="6" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
+      <c r="A9" s="8"/>
+      <c r="B9" s="8"/>
       <c r="C9" s="6" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C10" s="6" t="s">
@@ -727,38 +727,38 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7"/>
+      <c r="A11" s="8"/>
+      <c r="B11" s="8"/>
       <c r="C11" s="6" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="7"/>
-      <c r="B12" s="7"/>
+      <c r="A12" s="8"/>
+      <c r="B12" s="8"/>
       <c r="C12" s="6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
+      <c r="A13" s="8"/>
+      <c r="B13" s="8"/>
       <c r="C13" s="6" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
+      <c r="A14" s="8"/>
+      <c r="B14" s="8"/>
       <c r="C14" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C15" s="6" t="s">
@@ -766,45 +766,45 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
+      <c r="A16" s="8"/>
+      <c r="B16" s="8"/>
       <c r="C16" s="6" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
+      <c r="A17" s="8"/>
+      <c r="B17" s="8"/>
       <c r="C17" s="6" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="7"/>
-      <c r="B18" s="7"/>
+      <c r="A18" s="8"/>
+      <c r="B18" s="8"/>
       <c r="C18" s="6" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="7"/>
-      <c r="B19" s="7"/>
+      <c r="A19" s="8"/>
+      <c r="B19" s="8"/>
       <c r="C19" s="6" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="7"/>
-      <c r="B20" s="7"/>
+      <c r="A20" s="8"/>
+      <c r="B20" s="8"/>
       <c r="C20" s="6" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B21" s="8" t="s">
         <v>80</v>
       </c>
       <c r="C21" s="6" t="s">
@@ -812,63 +812,63 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="7"/>
-      <c r="B22" s="7"/>
+      <c r="A22" s="8"/>
+      <c r="B22" s="8"/>
       <c r="C22" s="6" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="7"/>
-      <c r="B23" s="7"/>
+      <c r="A23" s="8"/>
+      <c r="B23" s="8"/>
       <c r="C23" s="6" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="7"/>
-      <c r="B24" s="7"/>
+      <c r="A24" s="8"/>
+      <c r="B24" s="8"/>
       <c r="C24" s="6" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B25" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="6" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="8"/>
       <c r="B26" s="8"/>
-      <c r="C26" s="2" t="s">
+      <c r="C26" s="6" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="8"/>
       <c r="B27" s="8"/>
-      <c r="C27" s="2" t="s">
+      <c r="C27" s="6" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="8"/>
       <c r="B28" s="8"/>
-      <c r="C28" s="2" t="s">
+      <c r="C28" s="6" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B29" s="8" t="s">
+      <c r="A29" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29" s="7" t="s">
         <v>45</v>
       </c>
       <c r="C29" s="2" t="s">
@@ -876,38 +876,38 @@
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="8"/>
-      <c r="B30" s="8"/>
+      <c r="A30" s="7"/>
+      <c r="B30" s="7"/>
       <c r="C30" s="2" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="8"/>
-      <c r="B31" s="8"/>
+      <c r="A31" s="7"/>
+      <c r="B31" s="7"/>
       <c r="C31" s="2" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" s="8"/>
-      <c r="B32" s="8"/>
+      <c r="A32" s="7"/>
+      <c r="B32" s="7"/>
       <c r="C32" s="2" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" s="8"/>
-      <c r="B33" s="8"/>
+      <c r="A33" s="7"/>
+      <c r="B33" s="7"/>
       <c r="C33" s="2" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" s="8" t="s">
+      <c r="A34" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B34" s="8" t="s">
+      <c r="B34" s="7" t="s">
         <v>51</v>
       </c>
       <c r="C34" s="2" t="s">
@@ -915,17 +915,17 @@
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="8"/>
-      <c r="B35" s="8"/>
+      <c r="A35" s="7"/>
+      <c r="B35" s="7"/>
       <c r="C35" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" s="8" t="s">
+      <c r="A36" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B36" s="8" t="s">
+      <c r="B36" s="7" t="s">
         <v>54</v>
       </c>
       <c r="C36" s="2" t="s">
@@ -933,31 +933,31 @@
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="8"/>
-      <c r="B37" s="8"/>
+      <c r="A37" s="7"/>
+      <c r="B37" s="7"/>
       <c r="C37" s="2" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" s="8"/>
-      <c r="B38" s="8"/>
+      <c r="A38" s="7"/>
+      <c r="B38" s="7"/>
       <c r="C38" s="2" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" s="8"/>
-      <c r="B39" s="8"/>
+      <c r="A39" s="7"/>
+      <c r="B39" s="7"/>
       <c r="C39" s="2" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" s="8" t="s">
+      <c r="A40" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B40" s="8" t="s">
+      <c r="B40" s="7" t="s">
         <v>59</v>
       </c>
       <c r="C40" s="2" t="s">
@@ -965,24 +965,24 @@
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" s="8"/>
-      <c r="B41" s="8"/>
+      <c r="A41" s="7"/>
+      <c r="B41" s="7"/>
       <c r="C41" s="2" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42" s="8"/>
-      <c r="B42" s="8"/>
+      <c r="A42" s="7"/>
+      <c r="B42" s="7"/>
       <c r="C42" s="2" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43" s="8" t="s">
+      <c r="A43" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B43" s="8" t="s">
+      <c r="B43" s="7" t="s">
         <v>63</v>
       </c>
       <c r="C43" s="2" t="s">
@@ -990,15 +990,15 @@
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A44" s="8"/>
-      <c r="B44" s="8"/>
+      <c r="A44" s="7"/>
+      <c r="B44" s="7"/>
       <c r="C44" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A45" s="8"/>
-      <c r="B45" s="8"/>
+      <c r="A45" s="7"/>
+      <c r="B45" s="7"/>
       <c r="C45" s="2" t="s">
         <v>22</v>
       </c>
@@ -1038,6 +1038,20 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="A5:A9"/>
+    <mergeCell ref="B5:B9"/>
+    <mergeCell ref="A10:A14"/>
+    <mergeCell ref="B10:B14"/>
+    <mergeCell ref="A15:A20"/>
+    <mergeCell ref="B15:B20"/>
+    <mergeCell ref="A25:A28"/>
+    <mergeCell ref="B25:B28"/>
+    <mergeCell ref="A29:A33"/>
+    <mergeCell ref="B29:B33"/>
+    <mergeCell ref="A21:A24"/>
+    <mergeCell ref="B21:B24"/>
     <mergeCell ref="A43:A45"/>
     <mergeCell ref="B43:B45"/>
     <mergeCell ref="A34:A35"/>
@@ -1046,20 +1060,6 @@
     <mergeCell ref="B36:B39"/>
     <mergeCell ref="A40:A42"/>
     <mergeCell ref="B40:B42"/>
-    <mergeCell ref="A15:A20"/>
-    <mergeCell ref="B15:B20"/>
-    <mergeCell ref="A25:A28"/>
-    <mergeCell ref="B25:B28"/>
-    <mergeCell ref="A29:A33"/>
-    <mergeCell ref="B29:B33"/>
-    <mergeCell ref="A21:A24"/>
-    <mergeCell ref="B21:B24"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="A5:A9"/>
-    <mergeCell ref="B5:B9"/>
-    <mergeCell ref="A10:A14"/>
-    <mergeCell ref="B10:B14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
classwork React props state form is added
</commit_message>
<xml_diff>
--- a/JS_React_Syllabus.xlsx
+++ b/JS_React_Syllabus.xlsx
@@ -341,10 +341,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -629,8 +629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34:C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -652,10 +652,10 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>26</v>
       </c>
       <c r="C2" s="6" t="s">
@@ -663,24 +663,24 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="8"/>
-      <c r="B3" s="8"/>
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
       <c r="C3" s="6" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="8"/>
-      <c r="B4" s="8"/>
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
       <c r="C4" s="6" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>30</v>
       </c>
       <c r="C5" s="6" t="s">
@@ -688,38 +688,38 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="8"/>
-      <c r="B6" s="8"/>
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
       <c r="C6" s="6" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="8"/>
-      <c r="B7" s="8"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
       <c r="C7" s="6" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
       <c r="C8" s="6" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
       <c r="C9" s="6" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="7" t="s">
         <v>33</v>
       </c>
       <c r="C10" s="6" t="s">
@@ -727,38 +727,38 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
       <c r="C11" s="6" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
       <c r="C12" s="6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="8"/>
-      <c r="B13" s="8"/>
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
       <c r="C13" s="6" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
+      <c r="A14" s="7"/>
+      <c r="B14" s="7"/>
       <c r="C14" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C15" s="6" t="s">
@@ -766,45 +766,45 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
+      <c r="A16" s="7"/>
+      <c r="B16" s="7"/>
       <c r="C16" s="6" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8"/>
+      <c r="A17" s="7"/>
+      <c r="B17" s="7"/>
       <c r="C17" s="6" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
       <c r="C18" s="6" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="8"/>
-      <c r="B19" s="8"/>
+      <c r="A19" s="7"/>
+      <c r="B19" s="7"/>
       <c r="C19" s="6" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="8"/>
-      <c r="B20" s="8"/>
+      <c r="A20" s="7"/>
+      <c r="B20" s="7"/>
       <c r="C20" s="6" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="8" t="s">
+      <c r="A21" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="7" t="s">
         <v>80</v>
       </c>
       <c r="C21" s="6" t="s">
@@ -812,31 +812,31 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="8"/>
-      <c r="B22" s="8"/>
+      <c r="A22" s="7"/>
+      <c r="B22" s="7"/>
       <c r="C22" s="6" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="8"/>
-      <c r="B23" s="8"/>
+      <c r="A23" s="7"/>
+      <c r="B23" s="7"/>
       <c r="C23" s="6" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="8"/>
-      <c r="B24" s="8"/>
+      <c r="A24" s="7"/>
+      <c r="B24" s="7"/>
       <c r="C24" s="6" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="8" t="s">
+      <c r="A25" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="B25" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C25" s="6" t="s">
@@ -844,22 +844,22 @@
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="8"/>
-      <c r="B26" s="8"/>
+      <c r="A26" s="7"/>
+      <c r="B26" s="7"/>
       <c r="C26" s="6" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="8"/>
-      <c r="B27" s="8"/>
+      <c r="A27" s="7"/>
+      <c r="B27" s="7"/>
       <c r="C27" s="6" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="8"/>
-      <c r="B28" s="8"/>
+      <c r="A28" s="7"/>
+      <c r="B28" s="7"/>
       <c r="C28" s="6" t="s">
         <v>44</v>
       </c>
@@ -871,43 +871,43 @@
       <c r="B29" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C29" s="6" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="7"/>
       <c r="B30" s="7"/>
-      <c r="C30" s="2" t="s">
+      <c r="C30" s="6" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="7"/>
       <c r="B31" s="7"/>
-      <c r="C31" s="2" t="s">
+      <c r="C31" s="6" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="7"/>
       <c r="B32" s="7"/>
-      <c r="C32" s="2" t="s">
+      <c r="C32" s="6" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="7"/>
       <c r="B33" s="7"/>
-      <c r="C33" s="2" t="s">
+      <c r="C33" s="6" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B34" s="7" t="s">
+      <c r="A34" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B34" s="8" t="s">
         <v>51</v>
       </c>
       <c r="C34" s="2" t="s">
@@ -915,17 +915,17 @@
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="7"/>
-      <c r="B35" s="7"/>
+      <c r="A35" s="8"/>
+      <c r="B35" s="8"/>
       <c r="C35" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" s="7" t="s">
+      <c r="A36" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B36" s="7" t="s">
+      <c r="B36" s="8" t="s">
         <v>54</v>
       </c>
       <c r="C36" s="2" t="s">
@@ -933,31 +933,31 @@
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="7"/>
-      <c r="B37" s="7"/>
+      <c r="A37" s="8"/>
+      <c r="B37" s="8"/>
       <c r="C37" s="2" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" s="7"/>
-      <c r="B38" s="7"/>
+      <c r="A38" s="8"/>
+      <c r="B38" s="8"/>
       <c r="C38" s="2" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" s="7"/>
-      <c r="B39" s="7"/>
+      <c r="A39" s="8"/>
+      <c r="B39" s="8"/>
       <c r="C39" s="2" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" s="7" t="s">
+      <c r="A40" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B40" s="7" t="s">
+      <c r="B40" s="8" t="s">
         <v>59</v>
       </c>
       <c r="C40" s="2" t="s">
@@ -965,24 +965,24 @@
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" s="7"/>
-      <c r="B41" s="7"/>
+      <c r="A41" s="8"/>
+      <c r="B41" s="8"/>
       <c r="C41" s="2" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42" s="7"/>
-      <c r="B42" s="7"/>
+      <c r="A42" s="8"/>
+      <c r="B42" s="8"/>
       <c r="C42" s="2" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43" s="7" t="s">
+      <c r="A43" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B43" s="7" t="s">
+      <c r="B43" s="8" t="s">
         <v>63</v>
       </c>
       <c r="C43" s="2" t="s">
@@ -990,15 +990,15 @@
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A44" s="7"/>
-      <c r="B44" s="7"/>
+      <c r="A44" s="8"/>
+      <c r="B44" s="8"/>
       <c r="C44" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A45" s="7"/>
-      <c r="B45" s="7"/>
+      <c r="A45" s="8"/>
+      <c r="B45" s="8"/>
       <c r="C45" s="2" t="s">
         <v>22</v>
       </c>
@@ -1038,12 +1038,14 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="A5:A9"/>
-    <mergeCell ref="B5:B9"/>
-    <mergeCell ref="A10:A14"/>
-    <mergeCell ref="B10:B14"/>
+    <mergeCell ref="A43:A45"/>
+    <mergeCell ref="B43:B45"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="B36:B39"/>
+    <mergeCell ref="A40:A42"/>
+    <mergeCell ref="B40:B42"/>
     <mergeCell ref="A15:A20"/>
     <mergeCell ref="B15:B20"/>
     <mergeCell ref="A25:A28"/>
@@ -1052,14 +1054,12 @@
     <mergeCell ref="B29:B33"/>
     <mergeCell ref="A21:A24"/>
     <mergeCell ref="B21:B24"/>
-    <mergeCell ref="A43:A45"/>
-    <mergeCell ref="B43:B45"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="A36:A39"/>
-    <mergeCell ref="B36:B39"/>
-    <mergeCell ref="A40:A42"/>
-    <mergeCell ref="B40:B42"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="A5:A9"/>
+    <mergeCell ref="B5:B9"/>
+    <mergeCell ref="A10:A14"/>
+    <mergeCell ref="B10:B14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
personal finance tracker and json-server examples are added in classworks_answer and react_basics folder respectively
</commit_message>
<xml_diff>
--- a/JS_React_Syllabus.xlsx
+++ b/JS_React_Syllabus.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="88">
   <si>
     <t>Day</t>
   </si>
@@ -240,30 +240,6 @@
     <t>TypeScript</t>
   </si>
   <si>
-    <t>v8</t>
-  </si>
-  <si>
-    <t>start</t>
-  </si>
-  <si>
-    <t>end</t>
-  </si>
-  <si>
-    <t>browser</t>
-  </si>
-  <si>
-    <t>event loop</t>
-  </si>
-  <si>
-    <t>file read</t>
-  </si>
-  <si>
-    <t>processing the data</t>
-  </si>
-  <si>
-    <t>sync</t>
-  </si>
-  <si>
     <t>Version Control: Git and GitHub</t>
   </si>
   <si>
@@ -280,13 +256,46 @@
   </si>
   <si>
     <t>CSS: Media Query</t>
+  </si>
+  <si>
+    <t>Day 14</t>
+  </si>
+  <si>
+    <t>Day 1: React Router (Introduction)</t>
+  </si>
+  <si>
+    <t>Day 2: React Router (Navigation and Pages)</t>
+  </si>
+  <si>
+    <t>Day 3: State and Error Management (Advanced State)</t>
+  </si>
+  <si>
+    <t>Day 4: State and Error Management (Error Handling)</t>
+  </si>
+  <si>
+    <t>Day 5: State and Error Management (Exception Handling)</t>
+  </si>
+  <si>
+    <t>Day 6: React Optimization and Testing (State Management)</t>
+  </si>
+  <si>
+    <t>Day 7: React Optimization and Testing (Testing)</t>
+  </si>
+  <si>
+    <t>Day 8: React Optimization and Testing (WebSockets)</t>
+  </si>
+  <si>
+    <t>Day 9: Redux and WebSockets (Redux)</t>
+  </si>
+  <si>
+    <t>Day 10: TypeScript and CRUD Operations</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -302,13 +311,59 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -320,14 +375,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -337,18 +391,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="2" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -630,7 +697,7 @@
   <dimension ref="A1:C48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34:C35"/>
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -640,404 +707,418 @@
     <col min="3" max="3" width="87.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="8" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="4" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="6" t="s">
+      <c r="A3" s="11"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="4" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="6" t="s">
+      <c r="A4" s="11"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="4" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="6" t="s">
+      <c r="A6" s="11"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="4" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="6" t="s">
+      <c r="A7" s="11"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="6" t="s">
+      <c r="A8" s="11"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="6" t="s">
+      <c r="A9" s="11"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="4" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="4" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="6" t="s">
+      <c r="A11" s="11"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="4" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="7"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="6" t="s">
+      <c r="A12" s="11"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="6" t="s">
+      <c r="A13" s="11"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="4" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="2" t="s">
+      <c r="A14" s="11"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="4" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="6" t="s">
-        <v>79</v>
+      <c r="A16" s="11"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="4" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="6" t="s">
+      <c r="A17" s="11"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="4" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="7"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="6" t="s">
+      <c r="A18" s="11"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="4" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="7"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="6" t="s">
+      <c r="A19" s="11"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="4" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="7"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="6" t="s">
+      <c r="A20" s="11"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="4" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>81</v>
+      <c r="B21" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="7"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="6" t="s">
-        <v>82</v>
+      <c r="A22" s="11"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="4" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="7"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="6" t="s">
-        <v>83</v>
+      <c r="A23" s="11"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="4" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="7"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="6" t="s">
-        <v>84</v>
+      <c r="A24" s="11"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="4" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="7" t="s">
+      <c r="A25" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="B25" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="4" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="7"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="6" t="s">
+      <c r="A26" s="11"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="4" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="7"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="6" t="s">
+      <c r="A27" s="11"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="4" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="7"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="6" t="s">
+      <c r="A28" s="11"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="4" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="7" t="s">
+      <c r="A29" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="B29" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="C29" s="4" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="7"/>
-      <c r="B30" s="7"/>
-      <c r="C30" s="6" t="s">
+      <c r="A30" s="11"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="4" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="7"/>
-      <c r="B31" s="7"/>
-      <c r="C31" s="6" t="s">
+      <c r="A31" s="11"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="12" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" s="7"/>
-      <c r="B32" s="7"/>
-      <c r="C32" s="6" t="s">
+      <c r="A32" s="11"/>
+      <c r="B32" s="11"/>
+      <c r="C32" s="4" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" s="7"/>
-      <c r="B33" s="7"/>
-      <c r="C33" s="6" t="s">
+      <c r="A33" s="11"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="12" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" s="8" t="s">
+      <c r="A34" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B34" s="8" t="s">
+      <c r="B34" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C34" s="4" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="8"/>
-      <c r="B35" s="8"/>
-      <c r="C35" s="2" t="s">
+      <c r="A35" s="11"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="4" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B36" s="8" t="s">
+      <c r="A36" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B36" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C36" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="8"/>
-      <c r="B37" s="8"/>
-      <c r="C37" s="2" t="s">
+      <c r="A37" s="10"/>
+      <c r="B37" s="10"/>
+      <c r="C37" s="1" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" s="8"/>
-      <c r="B38" s="8"/>
-      <c r="C38" s="2" t="s">
+      <c r="A38" s="10"/>
+      <c r="B38" s="10"/>
+      <c r="C38" s="1" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" s="8"/>
-      <c r="B39" s="8"/>
-      <c r="C39" s="2" t="s">
+      <c r="A39" s="10"/>
+      <c r="B39" s="10"/>
+      <c r="C39" s="1" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B40" s="8" t="s">
+      <c r="A40" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B40" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C40" s="1" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" s="8"/>
-      <c r="B41" s="8"/>
-      <c r="C41" s="2" t="s">
+      <c r="A41" s="10"/>
+      <c r="B41" s="10"/>
+      <c r="C41" s="1" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42" s="8"/>
-      <c r="B42" s="8"/>
-      <c r="C42" s="2" t="s">
+      <c r="A42" s="10"/>
+      <c r="B42" s="10"/>
+      <c r="C42" s="1" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B43" s="8" t="s">
+      <c r="A43" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B43" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="C43" s="1" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A44" s="8"/>
-      <c r="B44" s="8"/>
-      <c r="C44" s="2" t="s">
+      <c r="A44" s="10"/>
+      <c r="B44" s="10"/>
+      <c r="C44" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A45" s="8"/>
-      <c r="B45" s="8"/>
-      <c r="C45" s="2" t="s">
+      <c r="A45" s="10"/>
+      <c r="B45" s="10"/>
+      <c r="C45" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A46" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B46" s="3" t="s">
+      <c r="A46" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B46" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="C46" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A47" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B47" s="3" t="s">
+      <c r="A47" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B47" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="C47" s="1" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>68</v>
-      </c>
-      <c r="B48" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B48" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C48" s="2" t="s">
+      <c r="C48" s="1" t="s">
         <v>67</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="A5:A9"/>
+    <mergeCell ref="B5:B9"/>
+    <mergeCell ref="A10:A14"/>
+    <mergeCell ref="B10:B14"/>
+    <mergeCell ref="A15:A20"/>
+    <mergeCell ref="B15:B20"/>
+    <mergeCell ref="A25:A28"/>
+    <mergeCell ref="B25:B28"/>
+    <mergeCell ref="A29:A33"/>
+    <mergeCell ref="B29:B33"/>
+    <mergeCell ref="A21:A24"/>
+    <mergeCell ref="B21:B24"/>
     <mergeCell ref="A43:A45"/>
     <mergeCell ref="B43:B45"/>
     <mergeCell ref="A34:A35"/>
@@ -1046,20 +1127,6 @@
     <mergeCell ref="B36:B39"/>
     <mergeCell ref="A40:A42"/>
     <mergeCell ref="B40:B42"/>
-    <mergeCell ref="A15:A20"/>
-    <mergeCell ref="B15:B20"/>
-    <mergeCell ref="A25:A28"/>
-    <mergeCell ref="B25:B28"/>
-    <mergeCell ref="A29:A33"/>
-    <mergeCell ref="B29:B33"/>
-    <mergeCell ref="A21:A24"/>
-    <mergeCell ref="B21:B24"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="A5:A9"/>
-    <mergeCell ref="B5:B9"/>
-    <mergeCell ref="A10:A14"/>
-    <mergeCell ref="B10:B14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1068,70 +1135,161 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A6:D20"/>
+  <dimension ref="A1:B42"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="16384" width="8.88671875" style="5"/>
+  </cols>
   <sheetData>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>1</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>2</v>
-      </c>
-      <c r="B8" t="s">
-        <v>76</v>
-      </c>
-      <c r="C8" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>3</v>
-      </c>
-      <c r="B9" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
-        <v>73</v>
-      </c>
-      <c r="D12">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
-        <v>71</v>
-      </c>
-      <c r="D14" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C18">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C20" t="s">
-        <v>75</v>
+      <c r="B1" s="6"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="7"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="7"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="7"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="7"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" s="7"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" s="7"/>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" s="6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" s="7"/>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32" s="7"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" s="7"/>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" s="7"/>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42" s="7" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
useReducer example is added
</commit_message>
<xml_diff>
--- a/JS_React_Syllabus.xlsx
+++ b/JS_React_Syllabus.xlsx
@@ -403,14 +403,14 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="2" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="2" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -697,7 +697,7 @@
   <dimension ref="A1:C48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -952,7 +952,7 @@
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="11"/>
       <c r="B31" s="11"/>
-      <c r="C31" s="12" t="s">
+      <c r="C31" s="10" t="s">
         <v>48</v>
       </c>
     </row>
@@ -966,7 +966,7 @@
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="11"/>
       <c r="B33" s="11"/>
-      <c r="C33" s="12" t="s">
+      <c r="C33" s="10" t="s">
         <v>50</v>
       </c>
     </row>
@@ -989,67 +989,67 @@
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" s="10" t="s">
+      <c r="A36" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B36" s="10" t="s">
+      <c r="B36" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C36" s="4" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="10"/>
-      <c r="B37" s="10"/>
-      <c r="C37" s="1" t="s">
+      <c r="A37" s="11"/>
+      <c r="B37" s="11"/>
+      <c r="C37" s="4" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" s="10"/>
-      <c r="B38" s="10"/>
-      <c r="C38" s="1" t="s">
+      <c r="A38" s="11"/>
+      <c r="B38" s="11"/>
+      <c r="C38" s="4" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" s="10"/>
-      <c r="B39" s="10"/>
-      <c r="C39" s="1" t="s">
+      <c r="A39" s="11"/>
+      <c r="B39" s="11"/>
+      <c r="C39" s="4" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" s="10" t="s">
+      <c r="A40" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B40" s="10" t="s">
+      <c r="B40" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C40" s="4" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" s="10"/>
-      <c r="B41" s="10"/>
-      <c r="C41" s="1" t="s">
+      <c r="A41" s="11"/>
+      <c r="B41" s="11"/>
+      <c r="C41" s="4" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42" s="10"/>
-      <c r="B42" s="10"/>
-      <c r="C42" s="1" t="s">
+      <c r="A42" s="11"/>
+      <c r="B42" s="11"/>
+      <c r="C42" s="4" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43" s="10" t="s">
+      <c r="A43" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="B43" s="10" t="s">
+      <c r="B43" s="12" t="s">
         <v>63</v>
       </c>
       <c r="C43" s="1" t="s">
@@ -1057,15 +1057,15 @@
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A44" s="10"/>
-      <c r="B44" s="10"/>
+      <c r="A44" s="12"/>
+      <c r="B44" s="12"/>
       <c r="C44" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A45" s="10"/>
-      <c r="B45" s="10"/>
+      <c r="A45" s="12"/>
+      <c r="B45" s="12"/>
       <c r="C45" s="1" t="s">
         <v>22</v>
       </c>
@@ -1105,12 +1105,14 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="A5:A9"/>
-    <mergeCell ref="B5:B9"/>
-    <mergeCell ref="A10:A14"/>
-    <mergeCell ref="B10:B14"/>
+    <mergeCell ref="A43:A45"/>
+    <mergeCell ref="B43:B45"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="B36:B39"/>
+    <mergeCell ref="A40:A42"/>
+    <mergeCell ref="B40:B42"/>
     <mergeCell ref="A15:A20"/>
     <mergeCell ref="B15:B20"/>
     <mergeCell ref="A25:A28"/>
@@ -1119,14 +1121,12 @@
     <mergeCell ref="B29:B33"/>
     <mergeCell ref="A21:A24"/>
     <mergeCell ref="B21:B24"/>
-    <mergeCell ref="A43:A45"/>
-    <mergeCell ref="B43:B45"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="A36:A39"/>
-    <mergeCell ref="B36:B39"/>
-    <mergeCell ref="A40:A42"/>
-    <mergeCell ref="B40:B42"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="A5:A9"/>
+    <mergeCell ref="B5:B9"/>
+    <mergeCell ref="A10:A14"/>
+    <mergeCell ref="B10:B14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
redux project and doc is added
</commit_message>
<xml_diff>
--- a/JS_React_Syllabus.xlsx
+++ b/JS_React_Syllabus.xlsx
@@ -406,10 +406,10 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="2" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -696,8 +696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -719,10 +719,10 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="12" t="s">
         <v>26</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -730,24 +730,24 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="11"/>
-      <c r="B3" s="11"/>
+      <c r="A3" s="12"/>
+      <c r="B3" s="12"/>
       <c r="C3" s="4" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="11"/>
-      <c r="B4" s="11"/>
+      <c r="A4" s="12"/>
+      <c r="B4" s="12"/>
       <c r="C4" s="4" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="12" t="s">
         <v>30</v>
       </c>
       <c r="C5" s="4" t="s">
@@ -755,38 +755,38 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11"/>
+      <c r="A6" s="12"/>
+      <c r="B6" s="12"/>
       <c r="C6" s="4" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11"/>
+      <c r="A7" s="12"/>
+      <c r="B7" s="12"/>
       <c r="C7" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="11"/>
-      <c r="B8" s="11"/>
+      <c r="A8" s="12"/>
+      <c r="B8" s="12"/>
       <c r="C8" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="11"/>
-      <c r="B9" s="11"/>
+      <c r="A9" s="12"/>
+      <c r="B9" s="12"/>
       <c r="C9" s="4" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="12" t="s">
         <v>33</v>
       </c>
       <c r="C10" s="4" t="s">
@@ -794,38 +794,38 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="11"/>
-      <c r="B11" s="11"/>
+      <c r="A11" s="12"/>
+      <c r="B11" s="12"/>
       <c r="C11" s="4" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="11"/>
-      <c r="B12" s="11"/>
+      <c r="A12" s="12"/>
+      <c r="B12" s="12"/>
       <c r="C12" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="11"/>
-      <c r="B13" s="11"/>
+      <c r="A13" s="12"/>
+      <c r="B13" s="12"/>
       <c r="C13" s="4" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="11"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="1" t="s">
+      <c r="A14" s="12"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="4" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="12" t="s">
         <v>6</v>
       </c>
       <c r="C15" s="4" t="s">
@@ -833,45 +833,45 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="11"/>
-      <c r="B16" s="11"/>
+      <c r="A16" s="12"/>
+      <c r="B16" s="12"/>
       <c r="C16" s="4" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="11"/>
-      <c r="B17" s="11"/>
+      <c r="A17" s="12"/>
+      <c r="B17" s="12"/>
       <c r="C17" s="4" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="11"/>
-      <c r="B18" s="11"/>
+      <c r="A18" s="12"/>
+      <c r="B18" s="12"/>
       <c r="C18" s="4" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="11"/>
-      <c r="B19" s="11"/>
+      <c r="A19" s="12"/>
+      <c r="B19" s="12"/>
       <c r="C19" s="4" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="11"/>
-      <c r="B20" s="11"/>
+      <c r="A20" s="12"/>
+      <c r="B20" s="12"/>
       <c r="C20" s="4" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="11" t="s">
+      <c r="A21" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="12" t="s">
         <v>72</v>
       </c>
       <c r="C21" s="4" t="s">
@@ -879,31 +879,31 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="11"/>
-      <c r="B22" s="11"/>
+      <c r="A22" s="12"/>
+      <c r="B22" s="12"/>
       <c r="C22" s="4" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="11"/>
-      <c r="B23" s="11"/>
+      <c r="A23" s="12"/>
+      <c r="B23" s="12"/>
       <c r="C23" s="4" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="11"/>
-      <c r="B24" s="11"/>
+      <c r="A24" s="12"/>
+      <c r="B24" s="12"/>
       <c r="C24" s="4" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="11" t="s">
+      <c r="A25" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B25" s="11" t="s">
+      <c r="B25" s="12" t="s">
         <v>8</v>
       </c>
       <c r="C25" s="4" t="s">
@@ -911,31 +911,31 @@
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="11"/>
-      <c r="B26" s="11"/>
+      <c r="A26" s="12"/>
+      <c r="B26" s="12"/>
       <c r="C26" s="4" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="11"/>
-      <c r="B27" s="11"/>
+      <c r="A27" s="12"/>
+      <c r="B27" s="12"/>
       <c r="C27" s="4" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="11"/>
-      <c r="B28" s="11"/>
+      <c r="A28" s="12"/>
+      <c r="B28" s="12"/>
       <c r="C28" s="4" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="11" t="s">
+      <c r="A29" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B29" s="11" t="s">
+      <c r="B29" s="12" t="s">
         <v>45</v>
       </c>
       <c r="C29" s="4" t="s">
@@ -943,38 +943,38 @@
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="11"/>
-      <c r="B30" s="11"/>
+      <c r="A30" s="12"/>
+      <c r="B30" s="12"/>
       <c r="C30" s="4" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="11"/>
-      <c r="B31" s="11"/>
+      <c r="A31" s="12"/>
+      <c r="B31" s="12"/>
       <c r="C31" s="10" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" s="11"/>
-      <c r="B32" s="11"/>
+      <c r="A32" s="12"/>
+      <c r="B32" s="12"/>
       <c r="C32" s="4" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" s="11"/>
-      <c r="B33" s="11"/>
+      <c r="A33" s="12"/>
+      <c r="B33" s="12"/>
       <c r="C33" s="10" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" s="11" t="s">
+      <c r="A34" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B34" s="11" t="s">
+      <c r="B34" s="12" t="s">
         <v>51</v>
       </c>
       <c r="C34" s="4" t="s">
@@ -982,17 +982,17 @@
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="11"/>
-      <c r="B35" s="11"/>
+      <c r="A35" s="12"/>
+      <c r="B35" s="12"/>
       <c r="C35" s="4" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" s="11" t="s">
+      <c r="A36" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B36" s="11" t="s">
+      <c r="B36" s="12" t="s">
         <v>54</v>
       </c>
       <c r="C36" s="4" t="s">
@@ -1000,31 +1000,31 @@
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="11"/>
-      <c r="B37" s="11"/>
+      <c r="A37" s="12"/>
+      <c r="B37" s="12"/>
       <c r="C37" s="4" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" s="11"/>
-      <c r="B38" s="11"/>
+      <c r="A38" s="12"/>
+      <c r="B38" s="12"/>
       <c r="C38" s="4" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" s="11"/>
-      <c r="B39" s="11"/>
+      <c r="A39" s="12"/>
+      <c r="B39" s="12"/>
       <c r="C39" s="4" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" s="11" t="s">
+      <c r="A40" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B40" s="11" t="s">
+      <c r="B40" s="12" t="s">
         <v>59</v>
       </c>
       <c r="C40" s="4" t="s">
@@ -1032,24 +1032,24 @@
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" s="11"/>
-      <c r="B41" s="11"/>
+      <c r="A41" s="12"/>
+      <c r="B41" s="12"/>
       <c r="C41" s="4" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42" s="11"/>
-      <c r="B42" s="11"/>
+      <c r="A42" s="12"/>
+      <c r="B42" s="12"/>
       <c r="C42" s="4" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43" s="12" t="s">
+      <c r="A43" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B43" s="12" t="s">
+      <c r="B43" s="11" t="s">
         <v>63</v>
       </c>
       <c r="C43" s="1" t="s">
@@ -1057,15 +1057,15 @@
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A44" s="12"/>
-      <c r="B44" s="12"/>
+      <c r="A44" s="11"/>
+      <c r="B44" s="11"/>
       <c r="C44" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A45" s="12"/>
-      <c r="B45" s="12"/>
+      <c r="A45" s="11"/>
+      <c r="B45" s="11"/>
       <c r="C45" s="1" t="s">
         <v>22</v>
       </c>
@@ -1105,6 +1105,20 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="A5:A9"/>
+    <mergeCell ref="B5:B9"/>
+    <mergeCell ref="A10:A14"/>
+    <mergeCell ref="B10:B14"/>
+    <mergeCell ref="A15:A20"/>
+    <mergeCell ref="B15:B20"/>
+    <mergeCell ref="A25:A28"/>
+    <mergeCell ref="B25:B28"/>
+    <mergeCell ref="A29:A33"/>
+    <mergeCell ref="B29:B33"/>
+    <mergeCell ref="A21:A24"/>
+    <mergeCell ref="B21:B24"/>
     <mergeCell ref="A43:A45"/>
     <mergeCell ref="B43:B45"/>
     <mergeCell ref="A34:A35"/>
@@ -1113,20 +1127,6 @@
     <mergeCell ref="B36:B39"/>
     <mergeCell ref="A40:A42"/>
     <mergeCell ref="B40:B42"/>
-    <mergeCell ref="A15:A20"/>
-    <mergeCell ref="B15:B20"/>
-    <mergeCell ref="A25:A28"/>
-    <mergeCell ref="B25:B28"/>
-    <mergeCell ref="A29:A33"/>
-    <mergeCell ref="B29:B33"/>
-    <mergeCell ref="A21:A24"/>
-    <mergeCell ref="B21:B24"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="A5:A9"/>
-    <mergeCell ref="B5:B9"/>
-    <mergeCell ref="A10:A14"/>
-    <mergeCell ref="B10:B14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>